<commit_message>
Reorganizing the file structure
</commit_message>
<xml_diff>
--- a/Assignment 6 CIELAB/MacbethColorChecker.xlsx
+++ b/Assignment 6 CIELAB/MacbethColorChecker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratheepkumarc/Documents/Development/Matlab/Principles-of-Color-Science/Assignment 6 CIELAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3DF020-ECAF-5443-AD9C-AE5CB5BB2A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CE0402-96EE-0F4F-B8A4-825561F60CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>wavelength</t>
-  </si>
-  <si>
-    <t>Patch Numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -68,10 +60,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,288 +146,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>500872</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="1027" name="Group 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF48629-A345-294B-B2F0-B87DE17852BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="18110200" y="165100"/>
-          <a:ext cx="4399772" cy="3124200"/>
-          <a:chOff x="1656" y="26"/>
-          <a:chExt cx="400" cy="246"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="1025" name="Picture 1">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166A33D6-E11F-A24D-883C-4614910B2F5A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1656" y="26"/>
-            <a:ext cx="351" cy="246"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="1026" name="Text Box 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E56F97D-A815-A04E-8D61-3F82FFC59C2D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1682" y="55"/>
-            <a:ext cx="374" cy="174"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-                <a:solidFill>
-                  <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                </a:solidFill>
-                <a:miter lim="800000"/>
-                <a:headEnd/>
-                <a:tailEnd/>
-              </a14:hiddenLine>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="none" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>1           2        3         4          5        6</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>7        8           9       10         11       12</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>13       14       15       16       17      18</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
-                <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>19      20        21        22       23       24       </a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA82"/>
+  <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -833,7 +542,7 @@
     <col min="2" max="25" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,11 +618,8 @@
       <c r="Y1">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>380</v>
       </c>
@@ -990,7 +696,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>385</v>
       </c>
@@ -1067,7 +773,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>390</v>
       </c>
@@ -1144,7 +850,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>395</v>
       </c>
@@ -1221,7 +927,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>400</v>
       </c>
@@ -1298,7 +1004,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>405</v>
       </c>
@@ -1375,7 +1081,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>410</v>
       </c>
@@ -1452,7 +1158,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>415</v>
       </c>
@@ -1529,7 +1235,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>420</v>
       </c>
@@ -1606,7 +1312,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>425</v>
       </c>
@@ -1683,7 +1389,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>430</v>
       </c>
@@ -1760,7 +1466,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>435</v>
       </c>
@@ -1837,7 +1543,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>440</v>
       </c>
@@ -1914,7 +1620,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>445</v>
       </c>
@@ -1991,7 +1697,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>450</v>
       </c>
@@ -7151,9 +6857,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>